<commit_message>
feat: Implement student management UI with CRUD operations and Excel import/export functionality.
</commit_message>
<xml_diff>
--- a/backend/templates/student-import-template.xlsx
+++ b/backend/templates/student-import-template.xlsx
@@ -1,11 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886F7EF1-4BCC-42D5-80A5-BC76C3919423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Students" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Instructions" state="visible" r:id="rId5"/>
+    <sheet name="Students" sheetId="1" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -110,9 +114,6 @@
     <t>2025-01-10</t>
   </si>
   <si>
-    <t>Grade 10</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -195,27 +196,33 @@
   </si>
   <si>
     <t>• If Class Name and Section are provided, Roll Number will be auto-generated</t>
+  </si>
+  <si>
+    <t>Grade 8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <color rgb="FFFFFFFF"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -587,9 +594,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
@@ -611,7 +623,7 @@
     <col min="23" max="23" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -682,7 +694,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -711,169 +723,172 @@
         <v>31</v>
       </c>
       <c r="J2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" t="s">
         <v>32</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>33</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>34</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>35</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>36</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>37</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>39</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>40</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>41</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>42</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>43</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>44</v>
-      </c>
-      <c r="W2" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A21"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="2" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>